<commit_message>
Little correction on some reported issues in "Eventos Cientificos".
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -585,7 +585,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{70CAFE08-6A16-4CDB-967D-D6D893EE6A58}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{834EC421-E264-4C87-A999-893F43D2E480}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Some little corrections on "Eventos" and "Redes" were added
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\CvLAC-Complete\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC-Complete\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1735B5-3BB1-4EC9-BD77-8AF32AF1DEC8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Documento</t>
   </si>
@@ -68,6 +69,15 @@
   </si>
   <si>
     <t>Departamento de Ingeniería Eléctrica y Electrónica</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000439185</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Adarme</t>
   </si>
 </sst>
 </file>
@@ -159,7 +169,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -582,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,18 +645,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>321</v>
+        <v>456</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>321</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -653,7 +681,8 @@
   <autoFilter ref="A1:E1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{834EC421-E264-4C87-A999-893F43D2E480}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{834EC421-E264-4C87-A999-893F43D2E480}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{5BE6EEC7-5619-4DD1-A624-5FAE0E9D15EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Issues with char: " on names were corrected.
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -52,9 +52,6 @@
     <t>Alarcon Guzman</t>
   </si>
   <si>
-    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000005410</t>
-  </si>
-  <si>
     <t>Departamento de ingeniería civil y agrícola</t>
   </si>
   <si>
@@ -68,13 +65,16 @@
   </si>
   <si>
     <t>Embus</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000218430</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -92,6 +92,14 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -146,11 +154,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -158,9 +167,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -571,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +624,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
         <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -624,16 +635,16 @@
         <v>321</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -642,6 +653,9 @@
       <sortCondition ref="E1"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{B11CAD1C-7E9D-4E96-8B40-AA70F37FF48D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>